<commit_message>
Cập nhật database và form main, login
</commit_message>
<xml_diff>
--- a/Phân công công việc qlns.xlsx
+++ b/Phân công công việc qlns.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\maithi\QLNS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -80,13 +80,13 @@
     <t>Xây dựng các module Thống kê nhân viên sắp nghỉ hưu, Thống kê nhân viên theo phòng, Thống kê sinh nhật tháng</t>
   </si>
   <si>
-    <t>Xây dựng các module Chấm công, Quản lí chức vụ, Khen thưởng kỷ luật                                       Ghép nối các module</t>
-  </si>
-  <si>
-    <t>Xây dựng các module, Thông tin gia đình, Thông tin Tài sản</t>
-  </si>
-  <si>
-    <t>Thiết kế giao diện đăng nhập, màn hình chính</t>
+    <t>Xây dựng các module Thông tin gia đình, Thông tin Tài sản</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xây dựng các module Chấm công, Quản lí chức vụ, Khen thưởng kỷ luật                                       </t>
+  </si>
+  <si>
+    <t>Thiết kế giao diện đăng nhập, màn hình chính, Ghép nối các module</t>
   </si>
 </sst>
 </file>
@@ -476,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -524,7 +524,7 @@
       </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" ht="49.2" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -577,34 +577,34 @@
         <v>6</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="42.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
         <v>7</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>5</v>
+      <c r="B10" s="14" t="s">
+        <v>18</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="10">
         <v>8</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="7"/>
     </row>

</xml_diff>